<commit_message>
Working version before neighborhood GIS regions
</commit_message>
<xml_diff>
--- a/Data/HVgrid Brabant.xlsx
+++ b/Data/HVgrid Brabant.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\Zenmo-Brabant-energiesysteem-V1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\Brabant-systeem-integratie-model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BFF646-B2CE-40A6-9B13-E902A88850A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D161E8-FAF9-420E-92DB-B96BAC371191}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -828,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1742,7 +1742,7 @@
         <v>90</v>
       </c>
       <c r="M22">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="N22">
         <v>46</v>

</xml_diff>